<commit_message>
added experiments in main text
</commit_message>
<xml_diff>
--- a/encodingTimeLargeSelectivityLargeMem.xlsx
+++ b/encodingTimeLargeSelectivityLargeMem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\Documents\Diplomatiki\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fotini\diplomatiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943A538A-A7C0-45F9-A481-68AF34D59D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF329AA-31BE-4BD8-A1C1-24ACE1275784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="465" yWindow="0" windowWidth="7500" windowHeight="6000" xr2:uid="{F4F57719-118F-45E0-A924-38EBED8242CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{F4F57719-118F-45E0-A924-38EBED8242CA}"/>
   </bookViews>
   <sheets>
     <sheet name="uniform" sheetId="1" r:id="rId1"/>
@@ -6786,19 +6786,19 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B2:B8"/>
+      <selection activeCell="A8" activeCellId="2" sqref="A6:XFD6 A7:XFD7 A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>10</v>
       </c>
@@ -6812,7 +6812,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>0.75700000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>7.1689999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>6.8879999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>178.36099999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>19.847000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>20.271000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -6945,16 +6945,16 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>10</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>7.8879999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>6.9539999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>14.205</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>24.195</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>27.215</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7101,16 +7101,16 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>10</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>0.45400000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>7.1660000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>7.1050000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>14.651999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>21.936</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7257,16 +7257,16 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>10</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>0.58399999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>7.0350000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>7.056</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>16.667999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>21.234999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>27.015999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>

</xml_diff>